<commit_message>
TMLE and LTMLE results with merged cohorts
</commit_message>
<xml_diff>
--- a/results/Paper/table_3.xlsx
+++ b/results/Paper/table_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\Race Disparities in Sepsis\mit-tmle\results\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F172EDA1-D5F4-4C7A-A096-984AC5DDD29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F3320E-63C4-4DDC-B388-B3F782D214F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMLE" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>cohort</t>
   </si>
@@ -57,9 +57,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>eICU</t>
-  </si>
-  <si>
     <t>ventilation_bin</t>
   </si>
   <si>
@@ -69,12 +66,6 @@
     <t>pressor</t>
   </si>
   <si>
-    <t>MIMIC</t>
-  </si>
-  <si>
-    <t>Cohort</t>
-  </si>
-  <si>
     <t>RRT</t>
   </si>
   <si>
@@ -105,10 +96,6 @@
     <t>Average Treatment Effect</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Ventilation</t>
-  </si>
-  <si>
     <t>i_ci</t>
   </si>
   <si>
@@ -119,6 +106,12 @@
   </si>
   <si>
     <t>r2</t>
+  </si>
+  <si>
+    <t>MIMIC_eICU</t>
+  </si>
+  <si>
+    <t>Ventilation</t>
   </si>
 </sst>
 </file>
@@ -643,12 +636,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1004,12 +997,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B29" sqref="B29"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:L31"/>
+      <selection pane="bottomLeft" activeCell="I16" activeCellId="1" sqref="O29 I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,37 +1012,37 @@
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
       <c r="M1"/>
@@ -1059,10 +1052,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1071,29 +1064,29 @@
         <v>100</v>
       </c>
       <c r="F2">
-        <v>-5.6390711380090497E-2</v>
+        <v>3.9649702705402197E-2</v>
       </c>
       <c r="G2">
-        <v>-6.8736929929353402E-2</v>
+        <v>3.24351404511182E-2</v>
       </c>
       <c r="H2">
-        <v>-4.4044492830827599E-2</v>
-      </c>
-      <c r="I2" s="9">
-        <v>3.4847286707252998E-19</v>
+        <v>4.6864264959686201E-2</v>
+      </c>
+      <c r="I2" s="8">
+        <v>4.6805037013071803E-27</v>
       </c>
       <c r="J2">
-        <v>0.77680723135540897</v>
+        <v>0.75862708018439395</v>
       </c>
       <c r="K2">
-        <v>0.15545642442086699</v>
+        <v>0.24074382928055699</v>
       </c>
       <c r="L2">
-        <v>27034</v>
+        <v>64971</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" ref="M2:M31" si="0">_xlfn.CONCAT(ROUND(F2, 2), " (", ROUND(G2,2), " - ", ROUND(H2,2),  ")", IF(AND(I2 &lt;0.05, NOT(ISBLANK(I2))), "*", " ") )</f>
-        <v>-0.06 (-0.07 - -0.04)*</v>
+        <v>0.04 (0.03 - 0.05)*</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1101,10 +1094,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1113,29 +1106,29 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>-4.5061376970214298E-2</v>
+        <v>5.6977266327060898E-2</v>
       </c>
       <c r="G3">
-        <v>-6.2967931187075304E-2</v>
+        <v>4.8266557102378899E-2</v>
       </c>
       <c r="H3">
-        <v>-2.7154822753353201E-2</v>
-      </c>
-      <c r="I3" s="9">
-        <v>8.1271586511145601E-7</v>
+        <v>6.5687975551742994E-2</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1.25924434821382E-37</v>
       </c>
       <c r="J3">
-        <v>0.71828202130138996</v>
+        <v>0.67951472062011697</v>
       </c>
       <c r="K3">
-        <v>0.14638151562014401</v>
+        <v>0.226828930680606</v>
       </c>
       <c r="L3">
-        <v>13301</v>
+        <v>38918</v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="0"/>
-        <v>-0.05 (-0.06 - -0.03)*</v>
+        <v>0.06 (0.05 - 0.07)*</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1143,10 +1136,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1155,29 +1148,29 @@
         <v>10</v>
       </c>
       <c r="F4">
-        <v>-5.2541601142769297E-2</v>
+        <v>3.0545574474793901E-2</v>
       </c>
       <c r="G4">
-        <v>-7.1558009065383205E-2</v>
+        <v>1.8003977030695801E-2</v>
       </c>
       <c r="H4">
-        <v>-3.3525193220155403E-2</v>
-      </c>
-      <c r="I4" s="9">
-        <v>6.1150354054404094E-8</v>
+        <v>4.3087171918891901E-2</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1.8090741817355399E-6</v>
       </c>
       <c r="J4">
-        <v>0.68559376125955196</v>
+        <v>0.68382649791566297</v>
       </c>
       <c r="K4">
-        <v>0.12618830015556301</v>
+        <v>0.169614629987135</v>
       </c>
       <c r="L4">
-        <v>10056</v>
+        <v>20375</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="0"/>
-        <v>-0.05 (-0.07 - -0.03)*</v>
+        <v>0.03 (0.02 - 0.04)*</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1185,10 +1178,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -1197,29 +1190,29 @@
         <v>15</v>
       </c>
       <c r="F5">
-        <v>-0.13618637563671099</v>
+        <v>-6.5420049782343698E-2</v>
       </c>
       <c r="G5">
-        <v>-0.175388023215959</v>
+        <v>-0.10019780625013899</v>
       </c>
       <c r="H5">
-        <v>-9.6984728057462596E-2</v>
-      </c>
-      <c r="I5" s="9">
-        <v>9.8257216137947493E-12</v>
+        <v>-3.06422933145486E-2</v>
+      </c>
+      <c r="I5">
+        <v>2.2697206982255099E-4</v>
       </c>
       <c r="J5">
-        <v>0.670631135278693</v>
+        <v>0.67272485220155998</v>
       </c>
       <c r="K5">
-        <v>8.5637493258098399E-2</v>
+        <v>8.5091333004247302E-2</v>
       </c>
       <c r="L5">
-        <v>3124</v>
+        <v>4963</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
-        <v>-0.14 (-0.18 - -0.1)*</v>
+        <v>-0.07 (-0.1 - -0.03)*</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1227,10 +1220,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>16</v>
@@ -1239,29 +1232,29 @@
         <v>100</v>
       </c>
       <c r="F6">
-        <v>-9.96236658628014E-2</v>
+        <v>-0.104989614788758</v>
       </c>
       <c r="G6">
-        <v>-0.214614804760104</v>
+        <v>-0.234486557580697</v>
       </c>
       <c r="H6">
-        <v>1.53674730345015E-2</v>
+        <v>2.450732800318E-2</v>
       </c>
       <c r="I6">
-        <v>8.9495565381075906E-2</v>
+        <v>0.11204469779836999</v>
       </c>
       <c r="J6">
-        <v>0.73637617209045803</v>
+        <v>0.71037630550904896</v>
       </c>
       <c r="K6">
-        <v>4.8799101255619398E-2</v>
+        <v>5.0420917798753503E-2</v>
       </c>
       <c r="L6">
-        <v>553</v>
+        <v>715</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">-0.1 (-0.21 - 0.02) </v>
+        <v xml:space="preserve">-0.1 (-0.23 - 0.02) </v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1269,10 +1262,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1281,29 +1274,29 @@
         <v>100</v>
       </c>
       <c r="F7">
-        <v>0.155139731147173</v>
+        <v>7.1007092336771993E-2</v>
       </c>
       <c r="G7">
-        <v>0.135162230519731</v>
+        <v>5.8813922844710403E-2</v>
       </c>
       <c r="H7">
-        <v>0.175117231774614</v>
-      </c>
-      <c r="I7" s="9">
-        <v>2.5729929262878002E-52</v>
+        <v>8.3200261828833597E-2</v>
+      </c>
+      <c r="I7" s="8">
+        <v>3.5561732572066498E-30</v>
       </c>
       <c r="J7">
-        <v>0.83121602151037599</v>
+        <v>0.79657059072427305</v>
       </c>
       <c r="K7">
-        <v>0.15507176794588201</v>
+        <v>0.240960893195061</v>
       </c>
       <c r="L7">
-        <v>27034</v>
+        <v>64971</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>0.16 (0.14 - 0.18)*</v>
+        <v>0.07 (0.06 - 0.08)*</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1311,10 +1304,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1323,29 +1316,29 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>0.20430310878864999</v>
+        <v>7.5490420970599895E-2</v>
       </c>
       <c r="G8">
-        <v>0.13410371051366099</v>
+        <v>4.5258512275272299E-2</v>
       </c>
       <c r="H8">
-        <v>0.27450250706363799</v>
-      </c>
-      <c r="I8" s="9">
-        <v>1.1686451887388299E-8</v>
+        <v>0.105722329665928</v>
+      </c>
+      <c r="I8" s="8">
+        <v>9.8702808510932501E-7</v>
       </c>
       <c r="J8">
-        <v>0.83064846259258696</v>
+        <v>0.74329582333512401</v>
       </c>
       <c r="K8">
-        <v>0.146777101266514</v>
+        <v>0.22760455580823399</v>
       </c>
       <c r="L8">
-        <v>13301</v>
+        <v>38918</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>0.2 (0.13 - 0.27)*</v>
+        <v>0.08 (0.05 - 0.11)*</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1353,10 +1346,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1365,29 +1358,29 @@
         <v>10</v>
       </c>
       <c r="F9">
-        <v>0.17067535295571401</v>
+        <v>8.6112103593664904E-2</v>
       </c>
       <c r="G9">
-        <v>0.13439187999073501</v>
+        <v>6.7402110527668799E-2</v>
       </c>
       <c r="H9">
-        <v>0.20695882592069401</v>
-      </c>
-      <c r="I9" s="9">
-        <v>2.97859394112861E-20</v>
+        <v>0.104822096659661</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1.86664440005519E-19</v>
       </c>
       <c r="J9">
-        <v>0.73291717575888904</v>
+        <v>0.68517516515953003</v>
       </c>
       <c r="K9">
-        <v>0.12512253293228401</v>
+        <v>0.16963347250173</v>
       </c>
       <c r="L9">
-        <v>10056</v>
+        <v>20375</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>0.17 (0.13 - 0.21)*</v>
+        <v>0.09 (0.07 - 0.1)*</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1395,10 +1388,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>11</v>
@@ -1407,29 +1400,29 @@
         <v>15</v>
       </c>
       <c r="F10">
-        <v>4.3691415977254199E-2</v>
+        <v>-1.04597027453155E-2</v>
       </c>
       <c r="G10">
-        <v>6.5372424310494899E-3</v>
+        <v>-4.0054537110019502E-2</v>
       </c>
       <c r="H10">
-        <v>8.0845589523458994E-2</v>
+        <v>1.9135131619388599E-2</v>
       </c>
       <c r="I10">
-        <v>2.1174405094428E-2</v>
+        <v>0.48848350975424198</v>
       </c>
       <c r="J10">
-        <v>0.66395161119580204</v>
+        <v>0.63694851284454501</v>
       </c>
       <c r="K10">
-        <v>8.5137814568928799E-2</v>
+        <v>8.3922101321058803E-2</v>
       </c>
       <c r="L10">
-        <v>3124</v>
+        <v>4963</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v>0.04 (0.01 - 0.08)*</v>
+        <v xml:space="preserve">-0.01 (-0.04 - 0.02) </v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1437,10 +1430,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -1449,29 +1442,29 @@
         <v>100</v>
       </c>
       <c r="F11">
-        <v>-6.0574365693823899E-2</v>
+        <v>-8.2957587135841199E-2</v>
       </c>
       <c r="G11">
-        <v>-0.13346486333893501</v>
+        <v>-0.146089177496456</v>
       </c>
       <c r="H11">
-        <v>1.2316131951287401E-2</v>
+        <v>-1.9825996775226701E-2</v>
       </c>
       <c r="I11">
-        <v>0.103350384686256</v>
+        <v>1.00088580670608E-2</v>
       </c>
       <c r="J11">
-        <v>0.62340579710144906</v>
+        <v>0.63889543284332095</v>
       </c>
       <c r="K11">
-        <v>5.2392830017636498E-2</v>
+        <v>5.4583121666331599E-2</v>
       </c>
       <c r="L11">
-        <v>553</v>
+        <v>715</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">-0.06 (-0.13 - 0.01) </v>
+        <v>-0.08 (-0.15 - -0.02)*</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1479,10 +1472,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1491,29 +1484,29 @@
         <v>100</v>
       </c>
       <c r="F12">
-        <v>-8.0890519550353396E-2</v>
+        <v>2.5972514110733601E-2</v>
       </c>
       <c r="G12">
-        <v>-9.4614537631098103E-2</v>
+        <v>1.8997744807534699E-2</v>
       </c>
       <c r="H12">
-        <v>-6.7166501469608605E-2</v>
-      </c>
-      <c r="I12" s="9">
-        <v>7.1782954943540698E-31</v>
+        <v>3.29472834139325E-2</v>
+      </c>
+      <c r="I12" s="8">
+        <v>2.9075368058534599E-13</v>
       </c>
       <c r="J12">
-        <v>0.81114063683878301</v>
+        <v>0.77251514698792101</v>
       </c>
       <c r="K12">
-        <v>0.15466326044720199</v>
+        <v>0.24087573669945</v>
       </c>
       <c r="L12">
-        <v>27034</v>
+        <v>64971</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
-        <v>-0.08 (-0.09 - -0.07)*</v>
+        <v>0.03 (0.02 - 0.03)*</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1521,10 +1514,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1533,29 +1526,29 @@
         <v>5</v>
       </c>
       <c r="F13">
-        <v>-8.9196963803291396E-2</v>
+        <v>1.98644593951137E-2</v>
       </c>
       <c r="G13">
-        <v>-0.106749038887385</v>
+        <v>1.1933737287247901E-2</v>
       </c>
       <c r="H13">
-        <v>-7.1644888719197497E-2</v>
-      </c>
-      <c r="I13" s="9">
-        <v>2.2710004747458301E-23</v>
+        <v>2.7795181502979601E-2</v>
+      </c>
+      <c r="I13" s="8">
+        <v>9.1399337693005304E-7</v>
       </c>
       <c r="J13">
-        <v>0.75020964778117605</v>
+        <v>0.67676292125549598</v>
       </c>
       <c r="K13">
-        <v>0.14721544080051999</v>
+        <v>0.22714844106232601</v>
       </c>
       <c r="L13">
-        <v>13301</v>
+        <v>38918</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
-        <v>-0.09 (-0.11 - -0.07)*</v>
+        <v>0.02 (0.01 - 0.03)*</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1563,10 +1556,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -1575,29 +1568,29 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <v>-9.1864003607172506E-2</v>
+        <v>1.8956391475746001E-2</v>
       </c>
       <c r="G14">
-        <v>-0.111443670929285</v>
+        <v>6.2648339082230203E-3</v>
       </c>
       <c r="H14">
-        <v>-7.2284336285060105E-2</v>
-      </c>
-      <c r="I14" s="9">
-        <v>3.7172985426127897E-20</v>
+        <v>3.1647949043269001E-2</v>
+      </c>
+      <c r="I14">
+        <v>3.4169970903865799E-3</v>
       </c>
       <c r="J14">
-        <v>0.69912542703615799</v>
+        <v>0.68383263415891005</v>
       </c>
       <c r="K14">
-        <v>0.125223863716246</v>
+        <v>0.16991992252252</v>
       </c>
       <c r="L14">
-        <v>10056</v>
+        <v>20375</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
-        <v>-0.09 (-0.11 - -0.07)*</v>
+        <v>0.02 (0.01 - 0.03)*</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1605,10 +1598,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1617,29 +1610,29 @@
         <v>15</v>
       </c>
       <c r="F15">
-        <v>-4.5685420807029002E-3</v>
+        <v>7.0131725466122799E-2</v>
       </c>
       <c r="G15">
-        <v>-6.1066732919472899E-2</v>
+        <v>2.23706386134498E-2</v>
       </c>
       <c r="H15">
-        <v>5.1929648758067097E-2</v>
+        <v>0.117892812318796</v>
       </c>
       <c r="I15">
-        <v>0.87407147793792705</v>
+        <v>4.0015802201711298E-3</v>
       </c>
       <c r="J15">
-        <v>0.72658124738568597</v>
+        <v>0.720549611660528</v>
       </c>
       <c r="K15">
-        <v>8.5662731960430394E-2</v>
+        <v>8.5860591318039206E-2</v>
       </c>
       <c r="L15">
-        <v>3124</v>
+        <v>4963</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0 (-0.06 - 0.05) </v>
+        <v>0.07 (0.02 - 0.12)*</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1647,10 +1640,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16">
         <v>16</v>
@@ -1659,650 +1652,29 @@
         <v>100</v>
       </c>
       <c r="F16">
-        <v>-8.3622020016262996E-2</v>
+        <v>-9.3087460280240494E-2</v>
       </c>
       <c r="G16">
-        <v>-0.21883476965863599</v>
+        <v>-0.227855576042444</v>
       </c>
       <c r="H16">
-        <v>5.1590729626109902E-2</v>
+        <v>4.1680655481962897E-2</v>
       </c>
       <c r="I16">
-        <v>0.225452066473289</v>
+        <v>0.17579463611688101</v>
       </c>
       <c r="J16">
-        <v>0.754235727440147</v>
+        <v>0.71978723404255296</v>
       </c>
       <c r="K16">
-        <v>5.7451058701775901E-2</v>
+        <v>5.1581000858653601E-2</v>
       </c>
       <c r="L16">
-        <v>553</v>
+        <v>715</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">-0.08 (-0.22 - 0.05) </v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-      <c r="F17">
-        <v>0.110680711479386</v>
-      </c>
-      <c r="G17">
-        <v>0.102086328293278</v>
-      </c>
-      <c r="H17">
-        <v>0.11927509466549301</v>
-      </c>
-      <c r="I17" s="9">
-        <v>1.4079566475126899E-140</v>
-      </c>
-      <c r="J17">
-        <v>0.74577062230885605</v>
-      </c>
-      <c r="K17">
-        <v>0.16840857658380701</v>
-      </c>
-      <c r="L17">
-        <v>37916</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="0"/>
-        <v>0.11 (0.1 - 0.12)*</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>0.112360073719854</v>
-      </c>
-      <c r="G18">
-        <v>0.10260229089294901</v>
-      </c>
-      <c r="H18">
-        <v>0.122117856546758</v>
-      </c>
-      <c r="I18" s="9">
-        <v>8.6926761115346005E-113</v>
-      </c>
-      <c r="J18">
-        <v>0.66395258224835996</v>
-      </c>
-      <c r="K18">
-        <v>0.127966786987294</v>
-      </c>
-      <c r="L18">
-        <v>25598</v>
-      </c>
-      <c r="M18" t="str">
-        <f t="shared" si="0"/>
-        <v>0.11 (0.1 - 0.12)*</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>6</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>0.113096934840501</v>
-      </c>
-      <c r="G19">
-        <v>9.6874664667429805E-2</v>
-      </c>
-      <c r="H19">
-        <v>0.129319205013573</v>
-      </c>
-      <c r="I19" s="9">
-        <v>1.65326752950212E-42</v>
-      </c>
-      <c r="J19">
-        <v>0.67727525300831604</v>
-      </c>
-      <c r="K19">
-        <v>8.6028577140750698E-2</v>
-      </c>
-      <c r="L19">
-        <v>10318</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" si="0"/>
-        <v>0.11 (0.1 - 0.13)*</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>11</v>
-      </c>
-      <c r="E20">
-        <v>15</v>
-      </c>
-      <c r="F20">
-        <v>4.8231291016371899E-2</v>
-      </c>
-      <c r="G20">
-        <v>-1.8737477965548099E-2</v>
-      </c>
-      <c r="H20">
-        <v>0.115200059998292</v>
-      </c>
-      <c r="I20">
-        <v>0.158066821750563</v>
-      </c>
-      <c r="J20">
-        <v>0.661940768746062</v>
-      </c>
-      <c r="K20">
-        <v>4.38236978699151E-2</v>
-      </c>
-      <c r="L20">
-        <v>1838</v>
-      </c>
-      <c r="M20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0.05 (-0.02 - 0.12) </v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21">
-        <v>16</v>
-      </c>
-      <c r="E21">
-        <v>100</v>
-      </c>
-      <c r="F21">
-        <v>-0.30001172798633302</v>
-      </c>
-      <c r="G21">
-        <v>-0.37120168245334001</v>
-      </c>
-      <c r="H21">
-        <v>-0.228821773519327</v>
-      </c>
-      <c r="I21" s="9">
-        <v>1.4577599680061E-16</v>
-      </c>
-      <c r="J21">
-        <v>0.5</v>
-      </c>
-      <c r="K21">
-        <v>5.8942263269760299E-2</v>
-      </c>
-      <c r="L21">
-        <v>162</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" si="0"/>
-        <v>-0.3 (-0.37 - -0.23)*</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>100</v>
-      </c>
-      <c r="F22">
-        <v>1.8008331886029801E-2</v>
-      </c>
-      <c r="G22">
-        <v>3.7692185321622799E-3</v>
-      </c>
-      <c r="H22">
-        <v>3.2247445239897303E-2</v>
-      </c>
-      <c r="I22">
-        <v>1.31814395933256E-2</v>
-      </c>
-      <c r="J22">
-        <v>0.77457721088577502</v>
-      </c>
-      <c r="K22">
-        <v>0.16881856552923999</v>
-      </c>
-      <c r="L22">
-        <v>37916</v>
-      </c>
-      <c r="M22" t="str">
-        <f t="shared" si="0"/>
-        <v>0.02 (0 - 0.03)*</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>5</v>
-      </c>
-      <c r="F23">
-        <v>3.1474579797553401E-2</v>
-      </c>
-      <c r="G23">
-        <v>4.8118862627518702E-3</v>
-      </c>
-      <c r="H23">
-        <v>5.8137273332355001E-2</v>
-      </c>
-      <c r="I23">
-        <v>2.0682737944244699E-2</v>
-      </c>
-      <c r="J23">
-        <v>0.71856728594963504</v>
-      </c>
-      <c r="K23">
-        <v>0.12676923147070901</v>
-      </c>
-      <c r="L23">
-        <v>25598</v>
-      </c>
-      <c r="M23" t="str">
-        <f t="shared" si="0"/>
-        <v>0.03 (0 - 0.06)*</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
-      </c>
-      <c r="F24">
-        <v>1.1560791459097899E-2</v>
-      </c>
-      <c r="G24">
-        <v>-1.0471494749317E-2</v>
-      </c>
-      <c r="H24">
-        <v>3.3593077667512801E-2</v>
-      </c>
-      <c r="I24">
-        <v>0.303737206565729</v>
-      </c>
-      <c r="J24">
-        <v>0.64052307791244401</v>
-      </c>
-      <c r="K24">
-        <v>8.63688566152018E-2</v>
-      </c>
-      <c r="L24">
-        <v>10318</v>
-      </c>
-      <c r="M24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0.01 (-0.01 - 0.03) </v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25">
-        <v>11</v>
-      </c>
-      <c r="E25">
-        <v>15</v>
-      </c>
-      <c r="F25">
-        <v>-0.107521010556945</v>
-      </c>
-      <c r="G25">
-        <v>-0.15677514663750999</v>
-      </c>
-      <c r="H25">
-        <v>-5.8266874476379897E-2</v>
-      </c>
-      <c r="I25" s="9">
-        <v>1.8803074839087401E-5</v>
-      </c>
-      <c r="J25">
-        <v>0.59655983373441202</v>
-      </c>
-      <c r="K25">
-        <v>4.8081251505667097E-2</v>
-      </c>
-      <c r="L25">
-        <v>1838</v>
-      </c>
-      <c r="M25" t="str">
-        <f t="shared" si="0"/>
-        <v>-0.11 (-0.16 - -0.06)*</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26">
-        <v>16</v>
-      </c>
-      <c r="E26">
-        <v>100</v>
-      </c>
-      <c r="F26">
-        <v>-0.14445720036774601</v>
-      </c>
-      <c r="G26">
-        <v>-0.28030058507850902</v>
-      </c>
-      <c r="H26">
-        <v>-8.61381565698352E-3</v>
-      </c>
-      <c r="I26">
-        <v>3.7134395749434501E-2</v>
-      </c>
-      <c r="J26">
-        <v>0.60950129632453898</v>
-      </c>
-      <c r="K26">
-        <v>5.1997886575744903E-2</v>
-      </c>
-      <c r="L26">
-        <v>162</v>
-      </c>
-      <c r="M26" t="str">
-        <f t="shared" si="0"/>
-        <v>-0.14 (-0.28 - -0.01)*</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>100</v>
-      </c>
-      <c r="F27">
-        <v>0.105980746818526</v>
-      </c>
-      <c r="G27">
-        <v>9.8275926381755099E-2</v>
-      </c>
-      <c r="H27">
-        <v>0.11368556725529699</v>
-      </c>
-      <c r="I27" s="9">
-        <v>4.35023632625184E-160</v>
-      </c>
-      <c r="J27">
-        <v>0.74459515041855295</v>
-      </c>
-      <c r="K27">
-        <v>0.16841458164704701</v>
-      </c>
-      <c r="L27">
-        <v>37916</v>
-      </c>
-      <c r="M27" t="str">
-        <f t="shared" si="0"/>
-        <v>0.11 (0.1 - 0.11)*</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>5</v>
-      </c>
-      <c r="F28">
-        <v>8.4448304480320396E-2</v>
-      </c>
-      <c r="G28">
-        <v>7.5933698947828907E-2</v>
-      </c>
-      <c r="H28">
-        <v>9.29629100128119E-2</v>
-      </c>
-      <c r="I28" s="9">
-        <v>3.5845164261057101E-84</v>
-      </c>
-      <c r="J28">
-        <v>0.64582140699617396</v>
-      </c>
-      <c r="K28">
-        <v>0.12681591469932699</v>
-      </c>
-      <c r="L28">
-        <v>25598</v>
-      </c>
-      <c r="M28" t="str">
-        <f t="shared" si="0"/>
-        <v>0.08 (0.08 - 0.09)*</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <v>10</v>
-      </c>
-      <c r="F29">
-        <v>0.13135169653439799</v>
-      </c>
-      <c r="G29">
-        <v>0.115347160962524</v>
-      </c>
-      <c r="H29">
-        <v>0.14735623210627299</v>
-      </c>
-      <c r="I29" s="9">
-        <v>3.1972769394527798E-58</v>
-      </c>
-      <c r="J29">
-        <v>0.66866675984704005</v>
-      </c>
-      <c r="K29">
-        <v>8.5345586841393595E-2</v>
-      </c>
-      <c r="L29">
-        <v>10318</v>
-      </c>
-      <c r="M29" t="str">
-        <f t="shared" si="0"/>
-        <v>0.13 (0.12 - 0.15)*</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30">
-        <v>11</v>
-      </c>
-      <c r="E30">
-        <v>15</v>
-      </c>
-      <c r="F30">
-        <v>0.210425482340237</v>
-      </c>
-      <c r="G30">
-        <v>0.124769800779852</v>
-      </c>
-      <c r="H30">
-        <v>0.296081163900621</v>
-      </c>
-      <c r="I30" s="9">
-        <v>1.4718406765388999E-6</v>
-      </c>
-      <c r="J30">
-        <v>0.70893757307419603</v>
-      </c>
-      <c r="K30">
-        <v>4.59323410491689E-2</v>
-      </c>
-      <c r="L30">
-        <v>1838</v>
-      </c>
-      <c r="M30" t="str">
-        <f t="shared" si="0"/>
-        <v>0.21 (0.12 - 0.3)*</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31">
-        <v>16</v>
-      </c>
-      <c r="E31">
-        <v>100</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>2.2193263262150199E-2</v>
-      </c>
-      <c r="L31">
-        <v>162</v>
-      </c>
-      <c r="M31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0 (0 - 0) </v>
+        <v xml:space="preserve">-0.09 (-0.23 - 0.04) </v>
       </c>
     </row>
   </sheetData>
@@ -2318,259 +1690,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:M23"/>
+  <dimension ref="B2:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="210" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
-    <col min="5" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.21875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="2" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
-      <c r="C5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
+      <c r="C5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>TMLE!M2</f>
+        <v>0.04 (0.03 - 0.05)*</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>TMLE!M2</f>
-        <v>-0.06 (-0.07 - -0.04)*</v>
+        <f>TMLE!M3</f>
+        <v>0.06 (0.05 - 0.07)*</v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>TMLE!M3</f>
-        <v>-0.05 (-0.06 - -0.03)*</v>
+        <f>TMLE!M4</f>
+        <v>0.03 (0.02 - 0.04)*</v>
       </c>
       <c r="G5" s="3" t="str">
-        <f>TMLE!M4</f>
-        <v>-0.05 (-0.07 - -0.03)*</v>
+        <f>TMLE!M5</f>
+        <v>-0.07 (-0.1 - -0.03)*</v>
       </c>
       <c r="H5" s="3" t="str">
-        <f>TMLE!M5</f>
-        <v>-0.14 (-0.18 - -0.1)*</v>
-      </c>
-      <c r="I5" s="3" t="str">
         <f>TMLE!M6</f>
-        <v xml:space="preserve">-0.1 (-0.21 - 0.02) </v>
-      </c>
+        <v xml:space="preserve">-0.1 (-0.23 - 0.02) </v>
+      </c>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>TMLE!M7</f>
+        <v>0.07 (0.06 - 0.08)*</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>TMLE!M7</f>
-        <v>0.16 (0.14 - 0.18)*</v>
-      </c>
-      <c r="F6" s="3" t="str">
         <f>TMLE!M8</f>
-        <v>0.2 (0.13 - 0.27)*</v>
-      </c>
-      <c r="G6" s="4" t="str">
+        <v>0.08 (0.05 - 0.11)*</v>
+      </c>
+      <c r="F6" s="4" t="str">
         <f>TMLE!M9</f>
-        <v>0.17 (0.13 - 0.21)*</v>
+        <v>0.09 (0.07 - 0.1)*</v>
+      </c>
+      <c r="G6" s="5" t="str">
+        <f>TMLE!M10</f>
+        <v xml:space="preserve">-0.01 (-0.04 - 0.02) </v>
       </c>
       <c r="H6" s="5" t="str">
-        <f>TMLE!M10</f>
-        <v>0.04 (0.01 - 0.08)*</v>
-      </c>
-      <c r="I6" s="5" t="str">
         <f>TMLE!M11</f>
-        <v xml:space="preserve">-0.06 (-0.13 - 0.01) </v>
-      </c>
+        <v>-0.08 (-0.15 - -0.02)*</v>
+      </c>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
-      <c r="C7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D7" s="3" t="str">
+        <f>TMLE!M12</f>
+        <v>0.03 (0.02 - 0.03)*</v>
+      </c>
       <c r="E7" s="3" t="str">
-        <f>TMLE!M12</f>
-        <v>-0.08 (-0.09 - -0.07)*</v>
+        <f>TMLE!M13</f>
+        <v>0.02 (0.01 - 0.03)*</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>TMLE!M13</f>
-        <v>-0.09 (-0.11 - -0.07)*</v>
+        <f>TMLE!M14</f>
+        <v>0.02 (0.01 - 0.03)*</v>
       </c>
       <c r="G7" s="3" t="str">
-        <f>TMLE!M14</f>
-        <v>-0.09 (-0.11 - -0.07)*</v>
+        <f>TMLE!M15</f>
+        <v>0.07 (0.02 - 0.12)*</v>
       </c>
       <c r="H7" s="3" t="str">
-        <f>TMLE!M15</f>
-        <v xml:space="preserve">0 (-0.06 - 0.05) </v>
-      </c>
-      <c r="I7" s="3" t="str">
         <f>TMLE!M16</f>
-        <v xml:space="preserve">-0.08 (-0.22 - 0.05) </v>
-      </c>
+        <v xml:space="preserve">-0.09 (-0.23 - 0.04) </v>
+      </c>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:12" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3" t="str">
-        <f>TMLE!M17</f>
-        <v>0.11 (0.1 - 0.12)*</v>
-      </c>
-      <c r="F8" s="3" t="str">
-        <f>TMLE!M18</f>
-        <v>0.11 (0.1 - 0.12)*</v>
-      </c>
-      <c r="G8" s="3" t="str">
-        <f>TMLE!M19</f>
-        <v>0.11 (0.1 - 0.13)*</v>
-      </c>
-      <c r="H8" s="3" t="str">
-        <f>TMLE!M20</f>
-        <v xml:space="preserve">0.05 (-0.02 - 0.12) </v>
-      </c>
-      <c r="I8" s="3" t="str">
-        <f>TMLE!M21</f>
-        <v>-0.3 (-0.37 - -0.23)*</v>
-      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="3" t="str">
-        <f>TMLE!M22</f>
-        <v>0.02 (0 - 0.03)*</v>
-      </c>
-      <c r="F9" s="3" t="str">
-        <f>TMLE!M23</f>
-        <v>0.03 (0 - 0.06)*</v>
-      </c>
-      <c r="G9" s="3" t="str">
-        <f>TMLE!M24</f>
-        <v xml:space="preserve">0.01 (-0.01 - 0.03) </v>
-      </c>
-      <c r="H9" s="3" t="str">
-        <f>TMLE!M25</f>
-        <v>-0.11 (-0.16 - -0.06)*</v>
-      </c>
-      <c r="I9" s="3" t="str">
-        <f>TMLE!M26</f>
-        <v>-0.14 (-0.28 - -0.01)*</v>
-      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="3" t="str">
-        <f>TMLE!M27</f>
-        <v>0.11 (0.1 - 0.11)*</v>
-      </c>
-      <c r="F10" s="3" t="str">
-        <f>TMLE!M28</f>
-        <v>0.08 (0.08 - 0.09)*</v>
-      </c>
-      <c r="G10" s="3" t="str">
-        <f>TMLE!M29</f>
-        <v>0.13 (0.12 - 0.15)*</v>
-      </c>
-      <c r="H10" s="3" t="str">
-        <f>TMLE!M30</f>
-        <v>0.21 (0.12 - 0.3)*</v>
-      </c>
-      <c r="I10" s="3" t="str">
-        <f>TMLE!M31</f>
-        <v xml:space="preserve">0 (0 - 0) </v>
-      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2582,11 +1889,10 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2596,9 +1902,8 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2610,9 +1915,8 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2624,9 +1928,8 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2638,9 +1941,8 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2652,9 +1954,8 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2666,9 +1967,8 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2680,9 +1980,8 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2694,9 +1993,8 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2708,57 +2006,10 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C3:D3"/>
+  <mergeCells count="1">
+    <mergeCell ref="D3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
TMLE results with corrected cohort
</commit_message>
<xml_diff>
--- a/results/Paper/table_3.xlsx
+++ b/results/Paper/table_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\Race Disparities in Sepsis\mit-tmle\results\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F3320E-63C4-4DDC-B388-B3F782D214F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0778C2F-5C30-4432-9E09-9880ED64F91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMLE" sheetId="1" r:id="rId1"/>
@@ -621,7 +621,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
@@ -640,6 +640,18 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1002,12 +1014,12 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B29" sqref="B29"/>
-      <selection pane="bottomLeft" activeCell="I16" activeCellId="1" sqref="O29 I16"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1064,29 +1076,29 @@
         <v>100</v>
       </c>
       <c r="F2">
-        <v>3.9649702705402197E-2</v>
+        <v>4.01060350675485E-2</v>
       </c>
       <c r="G2">
-        <v>3.24351404511182E-2</v>
+        <v>3.2911378046497998E-2</v>
       </c>
       <c r="H2">
-        <v>4.6864264959686201E-2</v>
+        <v>4.7300692088599099E-2</v>
       </c>
       <c r="I2" s="8">
-        <v>4.6805037013071803E-27</v>
+        <v>8.6713243938294297E-28</v>
       </c>
       <c r="J2">
-        <v>0.75862708018439395</v>
+        <v>0.75865806101890398</v>
       </c>
       <c r="K2">
-        <v>0.24074382928055699</v>
+        <v>0.240771376723381</v>
       </c>
       <c r="L2">
-        <v>64971</v>
+        <v>65301</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M31" si="0">_xlfn.CONCAT(ROUND(F2, 2), " (", ROUND(G2,2), " - ", ROUND(H2,2),  ")", IF(AND(I2 &lt;0.05, NOT(ISBLANK(I2))), "*", " ") )</f>
-        <v>0.04 (0.03 - 0.05)*</v>
+        <f>_xlfn.CONCAT(FIXED(F2, 3), " (", FIXED(G2,3), " to ", FIXED(H2,3),  ")", IF(AND(I2 &lt;0.05, NOT(ISBLANK(I2))), "*", " ") )</f>
+        <v>0.040 (0.033 to 0.047)*</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1106,29 +1118,29 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>5.6977266327060898E-2</v>
+        <v>5.718950394175E-2</v>
       </c>
       <c r="G3">
-        <v>4.8266557102378899E-2</v>
+        <v>4.8518170561639103E-2</v>
       </c>
       <c r="H3">
-        <v>6.5687975551742994E-2</v>
+        <v>6.5860837321860793E-2</v>
       </c>
       <c r="I3" s="8">
-        <v>1.25924434821382E-37</v>
+        <v>3.1832714466089599E-38</v>
       </c>
       <c r="J3">
-        <v>0.67951472062011697</v>
+        <v>0.67956226301494604</v>
       </c>
       <c r="K3">
-        <v>0.226828930680606</v>
+        <v>0.22739042344831201</v>
       </c>
       <c r="L3">
-        <v>38918</v>
+        <v>39158</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" si="0"/>
-        <v>0.06 (0.05 - 0.07)*</v>
+        <f t="shared" ref="M3:M16" si="0">_xlfn.CONCAT(FIXED(F3, 3), " (", FIXED(G3,3), " to ", FIXED(H3,3),  ")", IF(AND(I3 &lt;0.05, NOT(ISBLANK(I3))), "*", " ") )</f>
+        <v>0.057 (0.049 to 0.066)*</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1148,29 +1160,29 @@
         <v>10</v>
       </c>
       <c r="F4">
-        <v>3.0545574474793901E-2</v>
+        <v>3.2028841465504797E-2</v>
       </c>
       <c r="G4">
-        <v>1.8003977030695801E-2</v>
+        <v>1.9484876478251201E-2</v>
       </c>
       <c r="H4">
-        <v>4.3087171918891901E-2</v>
+        <v>4.45728064527584E-2</v>
       </c>
       <c r="I4" s="8">
-        <v>1.8090741817355399E-6</v>
+        <v>5.6001267696362001E-7</v>
       </c>
       <c r="J4">
-        <v>0.68382649791566297</v>
+        <v>0.68394877198026405</v>
       </c>
       <c r="K4">
-        <v>0.169614629987135</v>
+        <v>0.16886477305686301</v>
       </c>
       <c r="L4">
-        <v>20375</v>
+        <v>20456</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="0"/>
-        <v>0.03 (0.02 - 0.04)*</v>
+        <v>0.032 (0.019 to 0.045)*</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1190,29 +1202,29 @@
         <v>15</v>
       </c>
       <c r="F5">
-        <v>-6.5420049782343698E-2</v>
+        <v>-6.3976527250849097E-2</v>
       </c>
       <c r="G5">
-        <v>-0.10019780625013899</v>
+        <v>-9.9608107154666101E-2</v>
       </c>
       <c r="H5">
-        <v>-3.06422933145486E-2</v>
+        <v>-2.83449473470321E-2</v>
       </c>
       <c r="I5">
-        <v>2.2697206982255099E-4</v>
+        <v>4.3288060875864301E-4</v>
       </c>
       <c r="J5">
-        <v>0.67272485220155998</v>
+        <v>0.67279965118269702</v>
       </c>
       <c r="K5">
-        <v>8.5091333004247302E-2</v>
+        <v>8.3075135755322799E-2</v>
       </c>
       <c r="L5">
-        <v>4963</v>
+        <v>4972</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
-        <v>-0.07 (-0.1 - -0.03)*</v>
+        <v>-0.064 (-0.100 to -0.028)*</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1232,29 +1244,29 @@
         <v>100</v>
       </c>
       <c r="F6">
-        <v>-0.104989614788758</v>
+        <v>-9.7926746186490707E-2</v>
       </c>
       <c r="G6">
-        <v>-0.234486557580697</v>
+        <v>-0.23240311230281599</v>
       </c>
       <c r="H6">
-        <v>2.450732800318E-2</v>
+        <v>3.6549619929834999E-2</v>
       </c>
       <c r="I6">
-        <v>0.11204469779836999</v>
+        <v>0.153497071866394</v>
       </c>
       <c r="J6">
-        <v>0.71037630550904896</v>
+        <v>0.711691780275851</v>
       </c>
       <c r="K6">
-        <v>5.0420917798753503E-2</v>
+        <v>4.9611961058284103E-2</v>
       </c>
       <c r="L6">
         <v>715</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">-0.1 (-0.23 - 0.02) </v>
+        <v xml:space="preserve">-0.098 (-0.232 to 0.037) </v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1274,29 +1286,29 @@
         <v>100</v>
       </c>
       <c r="F7">
-        <v>7.1007092336771993E-2</v>
+        <v>7.1508026976911096E-2</v>
       </c>
       <c r="G7">
-        <v>5.8813922844710403E-2</v>
+        <v>5.9340425537583598E-2</v>
       </c>
       <c r="H7">
-        <v>8.3200261828833597E-2</v>
+        <v>8.3675628416238601E-2</v>
       </c>
       <c r="I7" s="8">
-        <v>3.5561732572066498E-30</v>
+        <v>1.0612197137132601E-30</v>
       </c>
       <c r="J7">
-        <v>0.79657059072427305</v>
+        <v>0.79651946276169905</v>
       </c>
       <c r="K7">
-        <v>0.240960893195061</v>
+        <v>0.24038940943374101</v>
       </c>
       <c r="L7">
-        <v>64971</v>
+        <v>65301</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>0.07 (0.06 - 0.08)*</v>
+        <v>0.072 (0.059 to 0.084)*</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1316,29 +1328,29 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>7.5490420970599895E-2</v>
+        <v>7.9342463988811798E-2</v>
       </c>
       <c r="G8">
-        <v>4.5258512275272299E-2</v>
+        <v>5.3593147248865901E-2</v>
       </c>
       <c r="H8">
-        <v>0.105722329665928</v>
+        <v>0.10509178072875799</v>
       </c>
       <c r="I8" s="8">
-        <v>9.8702808510932501E-7</v>
+        <v>1.5465834456572599E-9</v>
       </c>
       <c r="J8">
-        <v>0.74329582333512401</v>
+        <v>0.743168899722496</v>
       </c>
       <c r="K8">
-        <v>0.22760455580823399</v>
+        <v>0.227293834361358</v>
       </c>
       <c r="L8">
-        <v>38918</v>
+        <v>39158</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>0.08 (0.05 - 0.11)*</v>
+        <v>0.079 (0.054 to 0.105)*</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1358,29 +1370,29 @@
         <v>10</v>
       </c>
       <c r="F9">
-        <v>8.6112103593664904E-2</v>
+        <v>8.5824641418443995E-2</v>
       </c>
       <c r="G9">
-        <v>6.7402110527668799E-2</v>
+        <v>6.7102125487231101E-2</v>
       </c>
       <c r="H9">
-        <v>0.104822096659661</v>
+        <v>0.104547157349657</v>
       </c>
       <c r="I9" s="8">
-        <v>1.86664440005519E-19</v>
+        <v>2.5942746120491398E-19</v>
       </c>
       <c r="J9">
-        <v>0.68517516515953003</v>
+        <v>0.68457770752075797</v>
       </c>
       <c r="K9">
-        <v>0.16963347250173</v>
+        <v>0.16929587996758899</v>
       </c>
       <c r="L9">
-        <v>20375</v>
+        <v>20456</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>0.09 (0.07 - 0.1)*</v>
+        <v>0.086 (0.067 to 0.105)*</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1400,29 +1412,29 @@
         <v>15</v>
       </c>
       <c r="F10">
-        <v>-1.04597027453155E-2</v>
+        <v>-9.1571898623145093E-3</v>
       </c>
       <c r="G10">
-        <v>-4.0054537110019502E-2</v>
+        <v>-3.8537070112716398E-2</v>
       </c>
       <c r="H10">
-        <v>1.9135131619388599E-2</v>
+        <v>2.0222690388087401E-2</v>
       </c>
       <c r="I10">
-        <v>0.48848350975424198</v>
+        <v>0.54126751358918501</v>
       </c>
       <c r="J10">
-        <v>0.63694851284454501</v>
+        <v>0.63713875640670803</v>
       </c>
       <c r="K10">
-        <v>8.3922101321058803E-2</v>
+        <v>8.3344528369441506E-2</v>
       </c>
       <c r="L10">
-        <v>4963</v>
+        <v>4972</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">-0.01 (-0.04 - 0.02) </v>
+        <v xml:space="preserve">-0.009 (-0.039 to 0.020) </v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1442,29 +1454,29 @@
         <v>100</v>
       </c>
       <c r="F11">
-        <v>-8.2957587135841199E-2</v>
+        <v>-8.3341152168461205E-2</v>
       </c>
       <c r="G11">
-        <v>-0.146089177496456</v>
+        <v>-0.14784708842295899</v>
       </c>
       <c r="H11">
-        <v>-1.9825996775226701E-2</v>
+        <v>-1.88352159139634E-2</v>
       </c>
       <c r="I11">
-        <v>1.00088580670608E-2</v>
+        <v>1.1331561159533101E-2</v>
       </c>
       <c r="J11">
-        <v>0.63889543284332095</v>
+        <v>0.63880119989948403</v>
       </c>
       <c r="K11">
-        <v>5.4583121666331599E-2</v>
+        <v>4.9473161897019599E-2</v>
       </c>
       <c r="L11">
         <v>715</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
-        <v>-0.08 (-0.15 - -0.02)*</v>
+        <v>-0.083 (-0.148 to -0.019)*</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1484,29 +1496,29 @@
         <v>100</v>
       </c>
       <c r="F12">
-        <v>2.5972514110733601E-2</v>
+        <v>2.6182562193391101E-2</v>
       </c>
       <c r="G12">
-        <v>1.8997744807534699E-2</v>
+        <v>1.9222536232897498E-2</v>
       </c>
       <c r="H12">
-        <v>3.29472834139325E-2</v>
+        <v>3.3142588153884697E-2</v>
       </c>
       <c r="I12" s="8">
-        <v>2.9075368058534599E-13</v>
+        <v>1.66551828541935E-13</v>
       </c>
       <c r="J12">
-        <v>0.77251514698792101</v>
+        <v>0.772203891330424</v>
       </c>
       <c r="K12">
-        <v>0.24087573669945</v>
+        <v>0.24081255040971</v>
       </c>
       <c r="L12">
-        <v>64971</v>
+        <v>65301</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
-        <v>0.03 (0.02 - 0.03)*</v>
+        <v>0.026 (0.019 to 0.033)*</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1526,29 +1538,29 @@
         <v>5</v>
       </c>
       <c r="F13">
-        <v>1.98644593951137E-2</v>
+        <v>1.99434175230573E-2</v>
       </c>
       <c r="G13">
-        <v>1.1933737287247901E-2</v>
+        <v>1.20535302373129E-2</v>
       </c>
       <c r="H13">
-        <v>2.7795181502979601E-2</v>
+        <v>2.7833304808801699E-2</v>
       </c>
       <c r="I13" s="8">
-        <v>9.1399337693005304E-7</v>
+        <v>7.2580267024873805E-7</v>
       </c>
       <c r="J13">
-        <v>0.67676292125549598</v>
+        <v>0.67674116461315603</v>
       </c>
       <c r="K13">
-        <v>0.22714844106232601</v>
+        <v>0.22756518943689399</v>
       </c>
       <c r="L13">
-        <v>38918</v>
+        <v>39158</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
-        <v>0.02 (0.01 - 0.03)*</v>
+        <v>0.020 (0.012 to 0.028)*</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1568,29 +1580,29 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <v>1.8956391475746001E-2</v>
+        <v>1.8867903175626002E-2</v>
       </c>
       <c r="G14">
-        <v>6.2648339082230203E-3</v>
+        <v>6.1971028946747201E-3</v>
       </c>
       <c r="H14">
-        <v>3.1647949043269001E-2</v>
+        <v>3.1538703456577201E-2</v>
       </c>
       <c r="I14">
-        <v>3.4169970903865799E-3</v>
+        <v>3.5159884388428699E-3</v>
       </c>
       <c r="J14">
-        <v>0.68383263415891005</v>
+        <v>0.68348808776096703</v>
       </c>
       <c r="K14">
-        <v>0.16991992252252</v>
+        <v>0.16920315927814</v>
       </c>
       <c r="L14">
-        <v>20375</v>
+        <v>20456</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
-        <v>0.02 (0.01 - 0.03)*</v>
+        <v>0.019 (0.006 to 0.032)*</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1610,29 +1622,29 @@
         <v>15</v>
       </c>
       <c r="F15">
-        <v>7.0131725466122799E-2</v>
+        <v>7.2524321620886997E-2</v>
       </c>
       <c r="G15">
-        <v>2.23706386134498E-2</v>
+        <v>2.3759477702362999E-2</v>
       </c>
       <c r="H15">
-        <v>0.117892812318796</v>
+        <v>0.12128916553941101</v>
       </c>
       <c r="I15">
-        <v>4.0015802201711298E-3</v>
+        <v>3.55731773750761E-3</v>
       </c>
       <c r="J15">
-        <v>0.720549611660528</v>
+        <v>0.72067550488049603</v>
       </c>
       <c r="K15">
-        <v>8.5860591318039206E-2</v>
+        <v>8.3156426984279497E-2</v>
       </c>
       <c r="L15">
-        <v>4963</v>
+        <v>4972</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
-        <v>0.07 (0.02 - 0.12)*</v>
+        <v>0.073 (0.024 to 0.121)*</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1652,29 +1664,29 @@
         <v>100</v>
       </c>
       <c r="F16">
-        <v>-9.3087460280240494E-2</v>
+        <v>-0.26349355444148498</v>
       </c>
       <c r="G16">
-        <v>-0.227855576042444</v>
+        <v>-0.54196907006852801</v>
       </c>
       <c r="H16">
-        <v>4.1680655481962897E-2</v>
+        <v>1.49819611855581E-2</v>
       </c>
       <c r="I16">
-        <v>0.17579463611688101</v>
+        <v>6.3660206290522894E-2</v>
       </c>
       <c r="J16">
-        <v>0.71978723404255296</v>
+        <v>0.5</v>
       </c>
       <c r="K16">
-        <v>5.1581000858653601E-2</v>
+        <v>5.2347020624317703E-2</v>
       </c>
       <c r="L16">
         <v>715</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">-0.09 (-0.23 - 0.04) </v>
+        <v xml:space="preserve">-0.263 (-0.542 to 0.015) </v>
       </c>
     </row>
   </sheetData>
@@ -1693,14 +1705,15 @@
   <dimension ref="B2:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="2.21875" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="8" width="15" customWidth="1"/>
+    <col min="4" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
     <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1755,23 +1768,23 @@
       </c>
       <c r="D5" s="3" t="str">
         <f>TMLE!M2</f>
-        <v>0.04 (0.03 - 0.05)*</v>
+        <v>0.040 (0.033 to 0.047)*</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>TMLE!M3</f>
-        <v>0.06 (0.05 - 0.07)*</v>
+        <v>0.057 (0.049 to 0.066)*</v>
       </c>
       <c r="F5" s="3" t="str">
         <f>TMLE!M4</f>
-        <v>0.03 (0.02 - 0.04)*</v>
+        <v>0.032 (0.019 to 0.045)*</v>
       </c>
       <c r="G5" s="3" t="str">
         <f>TMLE!M5</f>
-        <v>-0.07 (-0.1 - -0.03)*</v>
+        <v>-0.064 (-0.100 to -0.028)*</v>
       </c>
       <c r="H5" s="3" t="str">
         <f>TMLE!M6</f>
-        <v xml:space="preserve">-0.1 (-0.23 - 0.02) </v>
+        <v xml:space="preserve">-0.098 (-0.232 to 0.037) </v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1785,23 +1798,23 @@
       </c>
       <c r="D6" s="3" t="str">
         <f>TMLE!M7</f>
-        <v>0.07 (0.06 - 0.08)*</v>
+        <v>0.072 (0.059 to 0.084)*</v>
       </c>
       <c r="E6" s="3" t="str">
         <f>TMLE!M8</f>
-        <v>0.08 (0.05 - 0.11)*</v>
+        <v>0.079 (0.054 to 0.105)*</v>
       </c>
       <c r="F6" s="4" t="str">
         <f>TMLE!M9</f>
-        <v>0.09 (0.07 - 0.1)*</v>
+        <v>0.086 (0.067 to 0.105)*</v>
       </c>
       <c r="G6" s="5" t="str">
         <f>TMLE!M10</f>
-        <v xml:space="preserve">-0.01 (-0.04 - 0.02) </v>
+        <v xml:space="preserve">-0.009 (-0.039 to 0.020) </v>
       </c>
       <c r="H6" s="5" t="str">
         <f>TMLE!M11</f>
-        <v>-0.08 (-0.15 - -0.02)*</v>
+        <v>-0.083 (-0.148 to -0.019)*</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1815,23 +1828,23 @@
       </c>
       <c r="D7" s="3" t="str">
         <f>TMLE!M12</f>
-        <v>0.03 (0.02 - 0.03)*</v>
+        <v>0.026 (0.019 to 0.033)*</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>TMLE!M13</f>
-        <v>0.02 (0.01 - 0.03)*</v>
+        <v>0.020 (0.012 to 0.028)*</v>
       </c>
       <c r="F7" s="3" t="str">
         <f>TMLE!M14</f>
-        <v>0.02 (0.01 - 0.03)*</v>
+        <v>0.019 (0.006 to 0.032)*</v>
       </c>
       <c r="G7" s="3" t="str">
         <f>TMLE!M15</f>
-        <v>0.07 (0.02 - 0.12)*</v>
+        <v>0.073 (0.024 to 0.121)*</v>
       </c>
       <c r="H7" s="3" t="str">
         <f>TMLE!M16</f>
-        <v xml:space="preserve">-0.09 (-0.23 - 0.04) </v>
+        <v xml:space="preserve">-0.263 (-0.542 to 0.015) </v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1879,12 +1892,12 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1892,12 +1905,12 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1905,12 +1918,12 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1918,12 +1931,12 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1931,12 +1944,12 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>

</xml_diff>

<commit_message>
TMLE results after corrected MIMIC cohort
</commit_message>
<xml_diff>
--- a/results/Paper/table_3.xlsx
+++ b/results/Paper/table_3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\Race Disparities in Sepsis\mit-tmle\results\Paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\TMLE\mit-tmle-sepsis\results\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0778C2F-5C30-4432-9E09-9880ED64F91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FD6F65-7CFA-414C-B97A-C329A4EC5AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -621,7 +621,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
@@ -638,22 +638,23 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1014,7 +1015,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B29" sqref="B29"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2:M16"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,77 +1024,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1"/>
-      <c r="B1" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="M1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="13">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="13">
         <v>100</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="13">
         <v>4.01060350675485E-2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="13">
         <v>3.2911378046497998E-2</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="13">
         <v>4.7300692088599099E-2</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="14">
         <v>8.6713243938294297E-28</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="13">
         <v>0.75865806101890398</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="13">
         <v>0.240771376723381</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="13">
         <v>65301</v>
       </c>
       <c r="M2" t="str">
@@ -1102,40 +1103,40 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="13">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="13">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="13">
         <v>5.718950394175E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="13">
         <v>4.8518170561639103E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="13">
         <v>6.5860837321860793E-2</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="14">
         <v>3.1832714466089599E-38</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="13">
         <v>0.67956226301494604</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="13">
         <v>0.22739042344831201</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="13">
         <v>39158</v>
       </c>
       <c r="M3" t="str">
@@ -1144,40 +1145,40 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="13">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="13">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="13">
         <v>3.2028841465504797E-2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="13">
         <v>1.9484876478251201E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="13">
         <v>4.45728064527584E-2</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="14">
         <v>5.6001267696362001E-7</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="13">
         <v>0.68394877198026405</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="13">
         <v>0.16886477305686301</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="13">
         <v>20456</v>
       </c>
       <c r="M4" t="str">
@@ -1186,40 +1187,40 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="13">
         <v>11</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="13">
         <v>15</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="13">
         <v>-6.3976527250849097E-2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="13">
         <v>-9.9608107154666101E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="13">
         <v>-2.83449473470321E-2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="13">
         <v>4.3288060875864301E-4</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="13">
         <v>0.67279965118269702</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="13">
         <v>8.3075135755322799E-2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="13">
         <v>4972</v>
       </c>
       <c r="M5" t="str">
@@ -1228,40 +1229,40 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="13">
         <v>16</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="13">
         <v>100</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="13">
         <v>-9.7926746186490707E-2</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="13">
         <v>-0.23240311230281599</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="13">
         <v>3.6549619929834999E-2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="13">
         <v>0.153497071866394</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="13">
         <v>0.711691780275851</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="13">
         <v>4.9611961058284103E-2</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="13">
         <v>715</v>
       </c>
       <c r="M6" t="str">
@@ -1270,40 +1271,40 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="13">
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="13">
         <v>100</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="13">
         <v>7.1508026976911096E-2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="13">
         <v>5.9340425537583598E-2</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="13">
         <v>8.3675628416238601E-2</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="14">
         <v>1.0612197137132601E-30</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="13">
         <v>0.79651946276169905</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="13">
         <v>0.24038940943374101</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="13">
         <v>65301</v>
       </c>
       <c r="M7" t="str">
@@ -1312,40 +1313,40 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="13">
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="13">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="13">
         <v>7.9342463988811798E-2</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="13">
         <v>5.3593147248865901E-2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="13">
         <v>0.10509178072875799</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="14">
         <v>1.5465834456572599E-9</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="13">
         <v>0.743168899722496</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="13">
         <v>0.227293834361358</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="13">
         <v>39158</v>
       </c>
       <c r="M8" t="str">
@@ -1354,40 +1355,40 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13">
         <v>6</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="13">
         <v>10</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="13">
         <v>8.5824641418443995E-2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="13">
         <v>6.7102125487231101E-2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="13">
         <v>0.104547157349657</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="14">
         <v>2.5942746120491398E-19</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="13">
         <v>0.68457770752075797</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="13">
         <v>0.16929587996758899</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="13">
         <v>20456</v>
       </c>
       <c r="M9" t="str">
@@ -1396,40 +1397,40 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="13">
         <v>11</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="13">
         <v>15</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="13">
         <v>-9.1571898623145093E-3</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="13">
         <v>-3.8537070112716398E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="13">
         <v>2.0222690388087401E-2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="13">
         <v>0.54126751358918501</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="13">
         <v>0.63713875640670803</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="13">
         <v>8.3344528369441506E-2</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="13">
         <v>4972</v>
       </c>
       <c r="M10" t="str">
@@ -1438,40 +1439,40 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="13">
         <v>16</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="13">
         <v>100</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="13">
         <v>-8.3341152168461205E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="13">
         <v>-0.14784708842295899</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="13">
         <v>-1.88352159139634E-2</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="13">
         <v>1.1331561159533101E-2</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="13">
         <v>0.63880119989948403</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="13">
         <v>4.9473161897019599E-2</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="13">
         <v>715</v>
       </c>
       <c r="M11" t="str">
@@ -1480,40 +1481,40 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="13">
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="13">
         <v>100</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="13">
         <v>2.6182562193391101E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="13">
         <v>1.9222536232897498E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="13">
         <v>3.3142588153884697E-2</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="14">
         <v>1.66551828541935E-13</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="13">
         <v>0.772203891330424</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="13">
         <v>0.24081255040971</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="13">
         <v>65301</v>
       </c>
       <c r="M12" t="str">
@@ -1522,40 +1523,40 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="13">
         <v>0</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="13">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="13">
         <v>1.99434175230573E-2</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="13">
         <v>1.20535302373129E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="13">
         <v>2.7833304808801699E-2</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="14">
         <v>7.2580267024873805E-7</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="13">
         <v>0.67674116461315603</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="13">
         <v>0.22756518943689399</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="13">
         <v>39158</v>
       </c>
       <c r="M13" t="str">
@@ -1564,40 +1565,40 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="13">
         <v>6</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="13">
         <v>10</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="13">
         <v>1.8867903175626002E-2</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="13">
         <v>6.1971028946747201E-3</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="13">
         <v>3.1538703456577201E-2</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="13">
         <v>3.5159884388428699E-3</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="13">
         <v>0.68348808776096703</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="13">
         <v>0.16920315927814</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="13">
         <v>20456</v>
       </c>
       <c r="M14" t="str">
@@ -1606,40 +1607,40 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="13">
         <v>11</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="13">
         <v>15</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="13">
         <v>7.2524321620886997E-2</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="13">
         <v>2.3759477702362999E-2</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="13">
         <v>0.12128916553941101</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="13">
         <v>3.55731773750761E-3</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="13">
         <v>0.72067550488049603</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="13">
         <v>8.3156426984279497E-2</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="13">
         <v>4972</v>
       </c>
       <c r="M15" t="str">
@@ -1648,40 +1649,40 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="13">
         <v>16</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="13">
         <v>100</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="13">
         <v>-0.26349355444148498</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="13">
         <v>-0.54196907006852801</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="13">
         <v>1.49819611855581E-2</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="13">
         <v>6.3660206290522894E-2</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="13">
         <v>0.5</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="13">
         <v>5.2347020624317703E-2</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="13">
         <v>715</v>
       </c>
       <c r="M16" t="str">
@@ -1704,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1724,13 +1725,13 @@
       <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1892,12 +1893,12 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1905,12 +1906,12 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1918,12 +1919,12 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1931,12 +1932,12 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1944,12 +1945,12 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>

</xml_diff>

<commit_message>
Plot TMLE results, python script and result
</commit_message>
<xml_diff>
--- a/results/Paper/table_3.xlsx
+++ b/results/Paper/table_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\TMLE\mit-tmle-sepsis\results\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FD6F65-7CFA-414C-B97A-C329A4EC5AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD64AFA-5C52-447D-8DE7-DFE8D38F36DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMLE" sheetId="1" r:id="rId1"/>
@@ -621,7 +621,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
@@ -650,11 +650,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1012,10 +1011,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B29" sqref="B29"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,77 +1023,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13" t="s">
+      <c r="A1"/>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
       <c r="M1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2">
         <v>100</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2">
         <v>4.01060350675485E-2</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2">
         <v>3.2911378046497998E-2</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2">
         <v>4.7300692088599099E-2</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="12">
         <v>8.6713243938294297E-28</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2">
         <v>0.75865806101890398</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2">
         <v>0.240771376723381</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2">
         <v>65301</v>
       </c>
       <c r="M2" t="str">
@@ -1103,40 +1102,40 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3">
         <v>5.718950394175E-2</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3">
         <v>4.8518170561639103E-2</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3">
         <v>6.5860837321860793E-2</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="12">
         <v>3.1832714466089599E-38</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3">
         <v>0.67956226301494604</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3">
         <v>0.22739042344831201</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3">
         <v>39158</v>
       </c>
       <c r="M3" t="str">
@@ -1145,40 +1144,40 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4">
         <v>6</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4">
         <v>3.2028841465504797E-2</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4">
         <v>1.9484876478251201E-2</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4">
         <v>4.45728064527584E-2</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="12">
         <v>5.6001267696362001E-7</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4">
         <v>0.68394877198026405</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4">
         <v>0.16886477305686301</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4">
         <v>20456</v>
       </c>
       <c r="M4" t="str">
@@ -1187,40 +1186,40 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5">
         <v>11</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5">
         <v>15</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5">
         <v>-6.3976527250849097E-2</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5">
         <v>-9.9608107154666101E-2</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5">
         <v>-2.83449473470321E-2</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5">
         <v>4.3288060875864301E-4</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5">
         <v>0.67279965118269702</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5">
         <v>8.3075135755322799E-2</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5">
         <v>4972</v>
       </c>
       <c r="M5" t="str">
@@ -1229,40 +1228,40 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6">
         <v>16</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6">
         <v>100</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6">
         <v>-9.7926746186490707E-2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6">
         <v>-0.23240311230281599</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6">
         <v>3.6549619929834999E-2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6">
         <v>0.153497071866394</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6">
         <v>0.711691780275851</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6">
         <v>4.9611961058284103E-2</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6">
         <v>715</v>
       </c>
       <c r="M6" t="str">
@@ -1271,40 +1270,40 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7">
         <v>100</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7">
         <v>7.1508026976911096E-2</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7">
         <v>5.9340425537583598E-2</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7">
         <v>8.3675628416238601E-2</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="12">
         <v>1.0612197137132601E-30</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7">
         <v>0.79651946276169905</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7">
         <v>0.24038940943374101</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7">
         <v>65301</v>
       </c>
       <c r="M7" t="str">
@@ -1313,40 +1312,40 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8">
         <v>7.9342463988811798E-2</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8">
         <v>5.3593147248865901E-2</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8">
         <v>0.10509178072875799</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="12">
         <v>1.5465834456572599E-9</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8">
         <v>0.743168899722496</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8">
         <v>0.227293834361358</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8">
         <v>39158</v>
       </c>
       <c r="M8" t="str">
@@ -1355,40 +1354,40 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9">
         <v>6</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9">
         <v>10</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9">
         <v>8.5824641418443995E-2</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9">
         <v>6.7102125487231101E-2</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9">
         <v>0.104547157349657</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="12">
         <v>2.5942746120491398E-19</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9">
         <v>0.68457770752075797</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9">
         <v>0.16929587996758899</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9">
         <v>20456</v>
       </c>
       <c r="M9" t="str">
@@ -1397,40 +1396,40 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10">
         <v>11</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10">
         <v>15</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10">
         <v>-9.1571898623145093E-3</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10">
         <v>-3.8537070112716398E-2</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10">
         <v>2.0222690388087401E-2</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10">
         <v>0.54126751358918501</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10">
         <v>0.63713875640670803</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10">
         <v>8.3344528369441506E-2</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10">
         <v>4972</v>
       </c>
       <c r="M10" t="str">
@@ -1439,40 +1438,40 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11">
         <v>16</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11">
         <v>100</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11">
         <v>-8.3341152168461205E-2</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11">
         <v>-0.14784708842295899</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11">
         <v>-1.88352159139634E-2</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11">
         <v>1.1331561159533101E-2</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11">
         <v>0.63880119989948403</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11">
         <v>4.9473161897019599E-2</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11">
         <v>715</v>
       </c>
       <c r="M11" t="str">
@@ -1481,40 +1480,40 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12">
         <v>100</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12">
         <v>2.6182562193391101E-2</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12">
         <v>1.9222536232897498E-2</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12">
         <v>3.3142588153884697E-2</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="12">
         <v>1.66551828541935E-13</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12">
         <v>0.772203891330424</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12">
         <v>0.24081255040971</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12">
         <v>65301</v>
       </c>
       <c r="M12" t="str">
@@ -1523,40 +1522,40 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13">
         <v>5</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13">
         <v>1.99434175230573E-2</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13">
         <v>1.20535302373129E-2</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13">
         <v>2.7833304808801699E-2</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="12">
         <v>7.2580267024873805E-7</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13">
         <v>0.67674116461315603</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13">
         <v>0.22756518943689399</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13">
         <v>39158</v>
       </c>
       <c r="M13" t="str">
@@ -1565,40 +1564,40 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14">
         <v>6</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14">
         <v>10</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14">
         <v>1.8867903175626002E-2</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14">
         <v>6.1971028946747201E-3</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14">
         <v>3.1538703456577201E-2</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14">
         <v>3.5159884388428699E-3</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14">
         <v>0.68348808776096703</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14">
         <v>0.16920315927814</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14">
         <v>20456</v>
       </c>
       <c r="M14" t="str">
@@ -1607,40 +1606,40 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15">
         <v>11</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15">
         <v>15</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15">
         <v>7.2524321620886997E-2</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15">
         <v>2.3759477702362999E-2</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15">
         <v>0.12128916553941101</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15">
         <v>3.55731773750761E-3</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15">
         <v>0.72067550488049603</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15">
         <v>8.3156426984279497E-2</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15">
         <v>4972</v>
       </c>
       <c r="M15" t="str">
@@ -1649,40 +1648,40 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16">
         <v>16</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16">
         <v>100</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16">
         <v>-0.26349355444148498</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16">
         <v>-0.54196907006852801</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16">
         <v>1.49819611855581E-2</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16">
         <v>6.3660206290522894E-2</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16">
         <v>0.5</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16">
         <v>5.2347020624317703E-2</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16">
         <v>715</v>
       </c>
       <c r="M16" t="str">
@@ -1705,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1725,13 +1724,13 @@
       <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>

</xml_diff>